<commit_message>
feat: remove loading data
</commit_message>
<xml_diff>
--- a/base/delivery_notes_January.xlsx
+++ b/base/delivery_notes_January.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,6 +590,64 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Product 5</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>40000.00</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>45680.98248739923</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>320000.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>17</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Product 6</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>80000.00</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>45681.35013923144</v>
+      </c>
+      <c r="F7" t="n">
+        <v>10</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>480000.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: change language to russian
</commit_message>
<xml_diff>
--- a/base/delivery_notes_January.xlsx
+++ b/base/delivery_notes_January.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -648,6 +648,93 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>18</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Product 7</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>60000.00</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>45681.37577218791</v>
+      </c>
+      <c r="F8" t="n">
+        <v>9</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>240000.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>19</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>fesfesfes</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>343434.00</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>45681.40553633918</v>
+      </c>
+      <c r="F9" t="n">
+        <v>11</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1717170.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>20</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Product 8</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>12430.00</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>45681.42420941254</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>12430.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>